<commit_message>
Adding investment agent with capacity to generate diversified portfolio. Updated app function to be more autonomous
</commit_message>
<xml_diff>
--- a/advice/config/general_investing_config.xlsx
+++ b/advice/config/general_investing_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ef78a42550bcb89/Documents/Learning/Ready Tensor/robo-advisor/advice/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="11_F25DC773A252ABDACC1048CB19DB428C5BDE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33AF2402-D689-4DC4-8407-ECADEA4945FB}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="11_F25DC773A252ABDACC1048CB19DB428C5BDE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0E60EB4-6743-45D0-8DD0-46739FBD81E7}"/>
   <bookViews>
-    <workbookView xWindow="-1370" yWindow="-20080" windowWidth="26360" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="372" yWindow="24" windowWidth="23016" windowHeight="12216" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Glidepath" sheetId="1" r:id="rId1"/>
@@ -111,6 +111,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,7 +382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -950,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6FDE3A-A055-437A-9E86-C1877407C41D}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -969,7 +973,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -977,7 +981,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -985,7 +989,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -993,7 +997,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>0.38</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1001,7 +1005,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>0.48</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1009,7 +1013,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1017,7 +1021,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>0.68</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1025,7 +1029,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>0.78</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1033,7 +1037,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>0.88</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1041,7 +1045,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>0.98</v>
+        <v>0.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>